<commit_message>
figures added, report annotated to point to file names
</commit_message>
<xml_diff>
--- a/assign2_results/assignment2_mb_results.xlsx
+++ b/assign2_results/assignment2_mb_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="6210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Serial MB" sheetId="2" r:id="rId1"/>
@@ -323,11 +323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42599552"/>
-        <c:axId val="42600128"/>
+        <c:axId val="56327488"/>
+        <c:axId val="120217600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42599552"/>
+        <c:axId val="56327488"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -368,12 +368,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42600128"/>
+        <c:crossAx val="120217600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42600128"/>
+        <c:axId val="120217600"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -420,7 +420,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42599552"/>
+        <c:crossAx val="56327488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -977,11 +977,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46483136"/>
-        <c:axId val="46483712"/>
+        <c:axId val="120979456"/>
+        <c:axId val="120980032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46483136"/>
+        <c:axId val="120979456"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1026,12 +1026,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46483712"/>
+        <c:crossAx val="120980032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46483712"/>
+        <c:axId val="120980032"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1078,7 +1078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46483136"/>
+        <c:crossAx val="120979456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1650,11 +1650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46486016"/>
-        <c:axId val="46486592"/>
+        <c:axId val="120982336"/>
+        <c:axId val="120982912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46486016"/>
+        <c:axId val="120982336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -1684,12 +1684,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46486592"/>
+        <c:crossAx val="120982912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46486592"/>
+        <c:axId val="120982912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46486016"/>
+        <c:crossAx val="120982336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2065,11 +2065,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46488896"/>
-        <c:axId val="106561536"/>
+        <c:axId val="120985216"/>
+        <c:axId val="120985792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46488896"/>
+        <c:axId val="120985216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2099,12 +2099,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106561536"/>
+        <c:crossAx val="120985792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106561536"/>
+        <c:axId val="120985792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2141,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46488896"/>
+        <c:crossAx val="120985216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -2468,11 +2468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106563840"/>
-        <c:axId val="106564416"/>
+        <c:axId val="121905728"/>
+        <c:axId val="121906304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106563840"/>
+        <c:axId val="121905728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2502,12 +2502,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106564416"/>
+        <c:crossAx val="121906304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106564416"/>
+        <c:axId val="121906304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2544,7 +2544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106563840"/>
+        <c:crossAx val="121905728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -2871,11 +2871,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106566720"/>
-        <c:axId val="106567296"/>
+        <c:axId val="121908608"/>
+        <c:axId val="121909184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106566720"/>
+        <c:axId val="121908608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -2905,12 +2905,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106567296"/>
+        <c:crossAx val="121909184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106567296"/>
+        <c:axId val="121909184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2947,7 +2947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106566720"/>
+        <c:crossAx val="121908608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -3091,11 +3091,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42601856"/>
-        <c:axId val="42602432"/>
+        <c:axId val="120219328"/>
+        <c:axId val="120219904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42601856"/>
+        <c:axId val="120219328"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3141,12 +3141,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42602432"/>
+        <c:crossAx val="120219904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42602432"/>
+        <c:axId val="120219904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3192,7 +3192,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42601856"/>
+        <c:crossAx val="120219328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3616,11 +3616,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42604160"/>
-        <c:axId val="42604736"/>
+        <c:axId val="120221632"/>
+        <c:axId val="120222208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42604160"/>
+        <c:axId val="120221632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3661,12 +3661,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42604736"/>
+        <c:crossAx val="120222208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42604736"/>
+        <c:axId val="120222208"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3711,7 +3711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42604160"/>
+        <c:crossAx val="120221632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4010,11 +4010,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45023808"/>
-        <c:axId val="45024384"/>
+        <c:axId val="120224512"/>
+        <c:axId val="120225088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45023808"/>
+        <c:axId val="120224512"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4061,12 +4061,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45024384"/>
+        <c:crossAx val="120225088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45024384"/>
+        <c:axId val="120225088"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -4111,7 +4111,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45023808"/>
+        <c:crossAx val="120224512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4392,11 +4392,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45026688"/>
-        <c:axId val="45027264"/>
+        <c:axId val="120702656"/>
+        <c:axId val="120703232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45026688"/>
+        <c:axId val="120702656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -4436,13 +4436,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45027264"/>
+        <c:crossAx val="120703232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45027264"/>
+        <c:axId val="120703232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4481,7 +4481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45026688"/>
+        <c:crossAx val="120702656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4763,11 +4763,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45029568"/>
-        <c:axId val="45030144"/>
+        <c:axId val="120705536"/>
+        <c:axId val="120706112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45029568"/>
+        <c:axId val="120705536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -4804,12 +4804,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45030144"/>
+        <c:crossAx val="120706112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45030144"/>
+        <c:axId val="120706112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -4839,7 +4839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45029568"/>
+        <c:crossAx val="120705536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -5106,11 +5106,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45966464"/>
-        <c:axId val="45967040"/>
+        <c:axId val="120708416"/>
+        <c:axId val="121085952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45966464"/>
+        <c:axId val="120708416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -5147,12 +5147,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45967040"/>
+        <c:crossAx val="121085952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45967040"/>
+        <c:axId val="121085952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5182,7 +5182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45966464"/>
+        <c:crossAx val="120708416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -5461,11 +5461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45969344"/>
-        <c:axId val="45969920"/>
+        <c:axId val="121088256"/>
+        <c:axId val="121088832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45969344"/>
+        <c:axId val="121088256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -5502,12 +5502,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45969920"/>
+        <c:crossAx val="121088832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45969920"/>
+        <c:axId val="121088832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -5537,7 +5537,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45969344"/>
+        <c:crossAx val="121088256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="25"/>
@@ -6163,11 +6163,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45972224"/>
-        <c:axId val="45972800"/>
+        <c:axId val="121091136"/>
+        <c:axId val="121091712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45972224"/>
+        <c:axId val="121091136"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6208,12 +6208,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45972800"/>
+        <c:crossAx val="121091712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45972800"/>
+        <c:axId val="121091712"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6260,7 +6260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45972224"/>
+        <c:crossAx val="121091136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7035,8 +7035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="E23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7213,8 +7213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M138"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G29"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8444,8 +8444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>